<commit_message>
Update after Excel Hidden Sheet name change
</commit_message>
<xml_diff>
--- a/Excel_Toolkit/Loadcases and combinations/Loadcases and Combinations.xlsx
+++ b/Excel_Toolkit/Loadcases and combinations/Loadcases and Combinations.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awakeman\Documents\My Received Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awakeman\code\BHoM\samples\Excel_Toolkit\Loadcases and combinations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11550" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="BHoM_Data" sheetId="3" state="hidden" r:id="rId1"/>
+    <sheet name="BHoM_DataHidden" sheetId="3" state="hidden" r:id="rId1"/>
     <sheet name="Loadcases" sheetId="1" r:id="rId2"/>
     <sheet name="Loads" sheetId="2" r:id="rId3"/>
     <sheet name="Load Combinations" sheetId="4" r:id="rId4"/>
@@ -177,8 +177,32 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Andrew Wakeman</author>
+  </authors>
+  <commentList>
+    <comment ref="F7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>This component failed to run properly. Inputs cannot be collected properly.
+Cannot convert type 'string' to 'BH.Adapter.BHoMAdapter'</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="95">
   <si>
     <t>Case #</t>
   </si>
@@ -429,43 +453,40 @@
     <t>{ "_t" : "BH.oM.Structure.Loads.AreaUniformalyDistributedLoad", "BHoM_Guid" : "9c3fae14-eccf-4a89-96de-eae28d73cf91", "Name" : "Wind West", "Tags" : [], "CustomData" : { }, "Loadcase" : { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "9cbbcf58-8562-4d3b-a574-35b16c49462b", "Name" : "Wind West", "Tags" : [], "CustomData" : { }, "Nature" : "Wind", "Number" : 6 }, "Objects" : { "_t" : "BH.oM.Base.BHoMGroup`1[[BH.oM.Structure.Elements.IAreaElement, Structure_oM, Version=1.0.0.0, Culture=neutral, PublicKeyToken=null]], BHoM, Version=1.0.0.0, Culture=neutral, PublicKeyToken=null", "BHoM_Guid" : "21956d90-484a-4a7c-9f1a-62f37227a91d", "Name" : "Wind West", "Tags" : [], "CustomData" : { }, "Elements" : [] }, "Axis" : "Global", "Projected" : false, "Pressure" : { "_t" : "BH.oM.Geometry.Vector", "X" : 1000.0, "Y" : 0.0, "Z" : 0.0 } }</t>
   </si>
   <si>
-    <t>{ "JNiynzx5" : { "_t" : "SocketAdapter", "AdapterId" : null, "BHoM_Guid" : "70277d24-d59e-4b7e-ad34-65edc9f02e12", "ErrorLog" : [] } }</t>
-  </si>
-  <si>
-    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "c7abadff-6d76-4c43-b10c-f8a61ea739a8", "Name" : "SLS Dead Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }]], "Number" : 100 }</t>
-  </si>
-  <si>
-    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "ba9322ae-1618-4ab1-91ed-81c5dcf276a4", "Name" : "SLS Super Imposed Dead Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }]], "Number" : 101 }</t>
-  </si>
-  <si>
-    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "6df2f5d7-3cfb-4a1e-b948-947d57398f9a", "Name" : "SLS Live Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "ac299599-0f0c-4233-b9d3-aa8b17d549a9", "Name" : "Live", "Tags" : [], "CustomData" : { }, "Nature" : "Live", "Number" : 3 }]], "Number" : 102 }</t>
-  </si>
-  <si>
-    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "36ac9421-7717-47b9-bee1-8e4a88a894e7", "Name" : "SLS Snow Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "c71e2a91-7ac9-49b8-a6b7-81de9c779af7", "Name" : "Snow", "Tags" : [], "CustomData" : { }, "Nature" : "Snow", "Number" : 4 }]], "Number" : 103 }</t>
-  </si>
-  <si>
-    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "e4732991-b860-4d78-9ac1-ccf9eff3b1aa", "Name" : "SLS Wind East", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "c02b7b1f-fb7d-4eae-8128-1ce2a6b3fcfd", "Name" : "Wind East", "Tags" : [], "CustomData" : { }, "Nature" : "Wind", "Number" : 5 }]], "Number" : 104 }</t>
-  </si>
-  <si>
-    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "1076c911-2e58-4131-ad91-e8ff2685fce7", "Name" : "SLS Wind West", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "9cbbcf58-8562-4d3b-a574-35b16c49462b", "Name" : "Wind West", "Tags" : [], "CustomData" : { }, "Nature" : "Wind", "Number" : 6 }]], "Number" : 105 }</t>
-  </si>
-  <si>
-    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "7ed618fc-96fc-44fb-93e7-44f0bb282052", "Name" : "ULS Dead Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }]], "Number" : 200 }</t>
-  </si>
-  <si>
-    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "0a24b3ef-d191-41dd-aa6e-879d143cc108", "Name" : "ULS Super Imposed Dead Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }]], "Number" : 201 }</t>
-  </si>
-  <si>
-    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "5072b5c2-4ab8-4d3c-a33b-18e5368f9420", "Name" : "ULS Live Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.6000000000000001, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "ac299599-0f0c-4233-b9d3-aa8b17d549a9", "Name" : "Live", "Tags" : [], "CustomData" : { }, "Nature" : "Live", "Number" : 3 }]], "Number" : 202 }</t>
-  </si>
-  <si>
-    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "3fa05d65-82c8-4d87-a2a1-a8ac40e7756a", "Name" : "ULS Snow Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.6000000000000001, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "c71e2a91-7ac9-49b8-a6b7-81de9c779af7", "Name" : "Snow", "Tags" : [], "CustomData" : { }, "Nature" : "Snow", "Number" : 4 }]], "Number" : 203 }</t>
-  </si>
-  <si>
-    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "96d1a66b-36f0-441e-99b1-a714980664da", "Name" : "ULS Wind East", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.6000000000000001, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "c02b7b1f-fb7d-4eae-8128-1ce2a6b3fcfd", "Name" : "Wind East", "Tags" : [], "CustomData" : { }, "Nature" : "Wind", "Number" : 5 }]], "Number" : 204 }</t>
-  </si>
-  <si>
-    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "de7d2920-73c7-40e6-8186-8b2fa139177f", "Name" : "ULS Wind West", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.6000000000000001, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "9cbbcf58-8562-4d3b-a574-35b16c49462b", "Name" : "Wind West", "Tags" : [], "CustomData" : { }, "Nature" : "Wind", "Number" : 6 }]], "Number" : 205 }</t>
+    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "9b55b667-b8ff-4df9-b807-2cb4c1846790", "Name" : "SLS Dead Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }]], "Number" : 100 }</t>
+  </si>
+  <si>
+    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "a95112f2-b32c-4b34-bd1c-c993594a95ff", "Name" : "SLS Super Imposed Dead Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }]], "Number" : 101 }</t>
+  </si>
+  <si>
+    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "65e64157-a6ea-481e-8cc7-d6a45bc8b569", "Name" : "SLS Live Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "ac299599-0f0c-4233-b9d3-aa8b17d549a9", "Name" : "Live", "Tags" : [], "CustomData" : { }, "Nature" : "Live", "Number" : 3 }]], "Number" : 102 }</t>
+  </si>
+  <si>
+    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "7f1e20a0-8b32-4c1e-96ce-990aefd1c257", "Name" : "SLS Snow Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "c71e2a91-7ac9-49b8-a6b7-81de9c779af7", "Name" : "Snow", "Tags" : [], "CustomData" : { }, "Nature" : "Snow", "Number" : 4 }]], "Number" : 103 }</t>
+  </si>
+  <si>
+    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "2c0f8a4c-bd73-41ac-9424-0dce219a953c", "Name" : "SLS Wind East", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "c02b7b1f-fb7d-4eae-8128-1ce2a6b3fcfd", "Name" : "Wind East", "Tags" : [], "CustomData" : { }, "Nature" : "Wind", "Number" : 5 }]], "Number" : 104 }</t>
+  </si>
+  <si>
+    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "57748cd8-2025-4fce-b8c7-13769ecd97f7", "Name" : "SLS Wind West", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.0, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "9cbbcf58-8562-4d3b-a574-35b16c49462b", "Name" : "Wind West", "Tags" : [], "CustomData" : { }, "Nature" : "Wind", "Number" : 6 }]], "Number" : 105 }</t>
+  </si>
+  <si>
+    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "3e9f6206-9a94-4a88-98bf-3c1b89ca5855", "Name" : "ULS Dead Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }]], "Number" : 200 }</t>
+  </si>
+  <si>
+    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "3dc37042-d4f6-469e-a0ee-d6ccddbc7ee9", "Name" : "ULS Super Imposed Dead Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }]], "Number" : 201 }</t>
+  </si>
+  <si>
+    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "14c6cbb2-a791-49cf-9161-dfc1a24c802d", "Name" : "ULS Live Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.6000000000000001, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "ac299599-0f0c-4233-b9d3-aa8b17d549a9", "Name" : "Live", "Tags" : [], "CustomData" : { }, "Nature" : "Live", "Number" : 3 }]], "Number" : 202 }</t>
+  </si>
+  <si>
+    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "3043b6fa-3cfe-4dc4-b44f-b89cf8727e7b", "Name" : "ULS Snow Load", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.6000000000000001, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "c71e2a91-7ac9-49b8-a6b7-81de9c779af7", "Name" : "Snow", "Tags" : [], "CustomData" : { }, "Nature" : "Snow", "Number" : 4 }]], "Number" : 203 }</t>
+  </si>
+  <si>
+    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "e3ac6d62-b51b-4e93-ad07-34865a544391", "Name" : "ULS Wind East", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.6000000000000001, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "c02b7b1f-fb7d-4eae-8128-1ce2a6b3fcfd", "Name" : "Wind East", "Tags" : [], "CustomData" : { }, "Nature" : "Wind", "Number" : 5 }]], "Number" : 204 }</t>
+  </si>
+  <si>
+    <t>{ "_t" : "BH.oM.Structure.Loads.LoadCombination", "BHoM_Guid" : "309d9d69-9df4-49d2-83dd-9f9b7e7bc84f", "Name" : "ULS Wind West", "Tags" : [], "CustomData" : { }, "LoadCases" : [[1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "d7869c88-52a5-4627-814f-a491ccbbe13f", "Name" : "Self-Weight", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 1 }], [1.3999999999999999, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "f9fdac07-a30e-429b-a4a9-514f52aba683", "Name" : "SDL", "Tags" : [], "CustomData" : { }, "Nature" : "Dead", "Number" : 2 }], [1.6000000000000001, { "_t" : "BH.oM.Structure.Loads.Loadcase", "BHoM_Guid" : "9cbbcf58-8562-4d3b-a574-35b16c49462b", "Name" : "Wind West", "Tags" : [], "CustomData" : { }, "Nature" : "Wind", "Number" : 6 }]], "Number" : 205 }</t>
   </si>
 </sst>
 </file>
@@ -553,7 +574,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -907,12 +928,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -989,6 +1030,25 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1016,28 +1076,18 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1319,7 +1369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1397,67 +1447,62 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1469,7 +1514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1492,7 +1537,7 @@
       <c r="D2" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="50" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="37" t="s">
@@ -1727,47 +1772,47 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="54" t="s">
+      <c r="B2" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="54" t="s">
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="54" t="s">
+      <c r="M2" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="54" t="s">
+      <c r="N2" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="54" t="s">
+      <c r="O2" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="50" t="s">
+      <c r="P2" s="63" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="53"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
       <c r="F3" s="38" t="s">
         <v>26</v>
       </c>
@@ -1786,11 +1831,11 @@
       <c r="K3" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="51"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="64"/>
       <c r="R3" s="37" t="s">
         <v>17</v>
       </c>
@@ -2528,7 +2573,7 @@
   <sheetData>
     <row r="1" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:26" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="70" t="str">
+      <c r="E2" s="60" t="str">
         <f ca="1">OFFSET(Loadcases!$C$3, COLUMN()-COLUMN($E$3), 0)</f>
         <v>Self-Weight</v>
       </c>
@@ -2569,7 +2614,7 @@
       <c r="Y2" s="19"/>
     </row>
     <row r="3" spans="2:26" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="71" t="str">
+      <c r="E3" s="61" t="str">
         <f ca="1">OFFSET(Loadcases!$D$3, COLUMN()-COLUMN($E$3), 0)</f>
         <v>Dead</v>
       </c>
@@ -2619,27 +2664,27 @@
       <c r="D4" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="69" t="str">
+      <c r="E4" s="59" t="str">
         <f ca="1">OFFSET(Loadcases!$E$3, COLUMN()-COLUMN($E$3), 0)</f>
         <v>Loadcase [iJyG16VS]</v>
       </c>
-      <c r="F4" s="64" t="str">
+      <c r="F4" s="54" t="str">
         <f ca="1">OFFSET(Loadcases!$E$3, COLUMN()-COLUMN($E$3), 0)</f>
         <v>Loadcase [B6z9+Q6j]</v>
       </c>
-      <c r="G4" s="69" t="str">
+      <c r="G4" s="59" t="str">
         <f ca="1">OFFSET(Loadcases!$E$3, COLUMN()-COLUMN($E$3), 0)</f>
         <v>Loadcase [mZUprAwP]</v>
       </c>
-      <c r="H4" s="64" t="str">
+      <c r="H4" s="54" t="str">
         <f ca="1">OFFSET(Loadcases!$E$3, COLUMN()-COLUMN($E$3), 0)</f>
         <v>Loadcase [kSoex8l6]</v>
       </c>
-      <c r="I4" s="69" t="str">
+      <c r="I4" s="59" t="str">
         <f ca="1">OFFSET(Loadcases!$E$3, COLUMN()-COLUMN($E$3), 0)</f>
         <v>Loadcase [H3srwH37]</v>
       </c>
-      <c r="J4" s="64" t="str">
+      <c r="J4" s="54" t="str">
         <f ca="1">OFFSET(Loadcases!$E$3, COLUMN()-COLUMN($E$3), 0)</f>
         <v>Loadcase [WM+7nGKF]</v>
       </c>
@@ -2660,49 +2705,49 @@
       <c r="Y4" s="23"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B5" s="65">
+      <c r="B5" s="55">
         <v>100</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="66" t="str">
+      <c r="D5" s="56" t="str">
         <f ca="1">_xll.Create.Structure.LoadCombination?by_String_Int32_ListOfLoadcase_ListOfDouble_Boolean(C5,B5,$E$4:$J$4,E5:J5)</f>
-        <v>LoadCombination [jm4usreV]</v>
-      </c>
-      <c r="E5" s="66">
+        <v>LoadCombination [HE4t/b9N]</v>
+      </c>
+      <c r="E5" s="56">
         <v>1</v>
       </c>
-      <c r="F5" s="67">
-        <v>0</v>
-      </c>
-      <c r="G5" s="66">
-        <v>0</v>
-      </c>
-      <c r="H5" s="67">
-        <v>0</v>
-      </c>
-      <c r="I5" s="66">
-        <v>0</v>
-      </c>
-      <c r="J5" s="67">
-        <v>0</v>
-      </c>
-      <c r="K5" s="66"/>
-      <c r="L5" s="67"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="67"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="67"/>
-      <c r="U5" s="66"/>
-      <c r="V5" s="67"/>
-      <c r="W5" s="66"/>
-      <c r="X5" s="67"/>
-      <c r="Y5" s="68"/>
+      <c r="F5" s="57">
+        <v>0</v>
+      </c>
+      <c r="G5" s="56">
+        <v>0</v>
+      </c>
+      <c r="H5" s="57">
+        <v>0</v>
+      </c>
+      <c r="I5" s="56">
+        <v>0</v>
+      </c>
+      <c r="J5" s="57">
+        <v>0</v>
+      </c>
+      <c r="K5" s="56"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="56"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="57"/>
+      <c r="U5" s="56"/>
+      <c r="V5" s="57"/>
+      <c r="W5" s="56"/>
+      <c r="X5" s="57"/>
+      <c r="Y5" s="58"/>
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
@@ -2714,7 +2759,7 @@
       </c>
       <c r="D6" s="27" t="str">
         <f ca="1">_xll.Create.Structure.LoadCombination?by_String_Int32_ListOfLoadcase_ListOfDouble_Boolean(C6,B6,$E$4:$J$4,E6:J6)</f>
-        <v>LoadCombination [YJLWV4R+]</v>
+        <v>LoadCombination [LB//9dpO]</v>
       </c>
       <c r="E6" s="27">
         <v>1</v>
@@ -2760,7 +2805,7 @@
       </c>
       <c r="D7" s="15" t="str">
         <f ca="1">_xll.Create.Structure.LoadCombination?by_String_Int32_ListOfLoadcase_ListOfDouble_Boolean(C7,B7,$E$4:$J$4,E7:J7)</f>
-        <v>LoadCombination [YEbNkDN6]</v>
+        <v>LoadCombination [TqBXtkZS]</v>
       </c>
       <c r="E7" s="15">
         <v>1</v>
@@ -2806,7 +2851,7 @@
       </c>
       <c r="D8" s="27" t="str">
         <f ca="1">_xll.Create.Structure.LoadCombination?by_String_Int32_ListOfLoadcase_ListOfDouble_Boolean(C8,B8,$E$4:$J$4,E8:J8)</f>
-        <v>LoadCombination [9vt6ABXh]</v>
+        <v>LoadCombination [BnwJfD9S]</v>
       </c>
       <c r="E8" s="27">
         <v>1</v>
@@ -2852,7 +2897,7 @@
       </c>
       <c r="D9" s="15" t="str">
         <f ca="1">_xll.Create.Structure.LoadCombination?by_String_Int32_ListOfLoadcase_ListOfDouble_Boolean(C9,B9,$E$4:$J$4,E9:J9)</f>
-        <v>LoadCombination [tSSkIWbg]</v>
+        <v>LoadCombination [ZaP+diSF]</v>
       </c>
       <c r="E9" s="15">
         <v>1</v>
@@ -2898,7 +2943,7 @@
       </c>
       <c r="D10" s="27" t="str">
         <f ca="1">_xll.Create.Structure.LoadCombination?by_String_Int32_ListOfLoadcase_ListOfDouble_Boolean(C10,B10,$E$4:$J$4,E10:J10)</f>
-        <v>LoadCombination [Phh+p6DF]</v>
+        <v>LoadCombination [cEbROykK]</v>
       </c>
       <c r="E10" s="27">
         <v>1</v>
@@ -2971,7 +3016,7 @@
       </c>
       <c r="D12" s="27" t="str">
         <f ca="1">_xll.Create.Structure.LoadCombination?by_String_Int32_ListOfLoadcase_ListOfDouble_Boolean(C12,B12,$E$4:$J$4,E12:J12)</f>
-        <v>LoadCombination [88TklhfL]</v>
+        <v>LoadCombination [IIjaNmlL]</v>
       </c>
       <c r="E12" s="27">
         <v>1.4</v>
@@ -3017,7 +3062,7 @@
       </c>
       <c r="D13" s="15" t="str">
         <f ca="1">_xll.Create.Structure.LoadCombination?by_String_Int32_ListOfLoadcase_ListOfDouble_Boolean(C13,B13,$E$4:$J$4,E13:J13)</f>
-        <v>LoadCombination [1VNKNGzI]</v>
+        <v>LoadCombination [4rQZIoTv]</v>
       </c>
       <c r="E13" s="15">
         <v>1.4</v>
@@ -3063,7 +3108,7 @@
       </c>
       <c r="D14" s="27" t="str">
         <f ca="1">_xll.Create.Structure.LoadCombination?by_String_Int32_ListOfLoadcase_ListOfDouble_Boolean(C14,B14,$E$4:$J$4,E14:J14)</f>
-        <v>LoadCombination [KtcEejd9]</v>
+        <v>LoadCombination [Zl6lO3t0]</v>
       </c>
       <c r="E14" s="27">
         <v>1.4</v>
@@ -3109,7 +3154,7 @@
       </c>
       <c r="D15" s="15" t="str">
         <f ca="1">_xll.Create.Structure.LoadCombination?by_String_Int32_ListOfLoadcase_ListOfDouble_Boolean(C15,B15,$E$4:$J$4,E15:J15)</f>
-        <v>LoadCombination [awe127Mx]</v>
+        <v>LoadCombination [lUEAftUD]</v>
       </c>
       <c r="E15" s="15">
         <v>1.4</v>
@@ -3155,7 +3200,7 @@
       </c>
       <c r="D16" s="27" t="str">
         <f ca="1">_xll.Create.Structure.LoadCombination?by_String_Int32_ListOfLoadcase_ListOfDouble_Boolean(C16,B16,$E$4:$J$4,E16:J16)</f>
-        <v>LoadCombination [Kr58W7r2]</v>
+        <v>LoadCombination [HlaRcV89]</v>
       </c>
       <c r="E16" s="27">
         <v>1.4</v>
@@ -3201,7 +3246,7 @@
       </c>
       <c r="D17" s="17" t="str">
         <f ca="1">_xll.Create.Structure.LoadCombination?by_String_Int32_ListOfLoadcase_ListOfDouble_Boolean(C17,B17,$E$4:$J$4,E17:J17)</f>
-        <v>LoadCombination [CPqcTd+d]</v>
+        <v>LoadCombination [KykA7SlI]</v>
       </c>
       <c r="E17" s="17">
         <v>1.4</v>
@@ -3248,11 +3293,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3264,26 +3309,26 @@
     <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1" s="59" t="s">
+    <row r="1" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="72" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="72" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="59"/>
+      <c r="F2" s="73"/>
     </row>
     <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="59"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="75"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="51" t="s">
         <v>60</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -3296,7 +3341,7 @@
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="52" t="s">
         <v>61</v>
       </c>
       <c r="C5" s="9">
@@ -3313,7 +3358,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="52" t="s">
         <v>62</v>
       </c>
       <c r="C6" s="9">
@@ -3330,7 +3375,7 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="53" t="s">
         <v>63</v>
       </c>
       <c r="C7" s="12">
@@ -3341,14 +3386,14 @@
         <f>_xll.Adapter.Create.SocketAdapter?by_String_Int32(,C7)</f>
         <v>SocketAdapter [JNiynzx5]</v>
       </c>
-      <c r="F7" s="13" t="b">
+      <c r="F7" s="13" t="e">
         <f ca="1">_xll.Adapter.Push?by_BHoMAdapter_IEnumerableOfIObject_String_DictionaryOfString_Object_Boolean(E7, 'Load Combinations'!D5:D17, , , $C$2)</f>
-        <v>0</v>
+        <v>#NULL!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="E2:F3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D2">
@@ -3357,5 +3402,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>